<commit_message>
CIERRE 18 ENE 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL#14  ARCHIVO  2 0 2 1/CENTRAL # 12  DICIEMBRE   2021/BALANCE    ZAVALETA   DICIEMBRE     2021.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL#14  ARCHIVO  2 0 2 1/CENTRAL # 12  DICIEMBRE   2021/BALANCE    ZAVALETA   DICIEMBRE     2021.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3690" yWindow="0" windowWidth="16605" windowHeight="10920" firstSheet="4" activeTab="5"/>
+    <workbookView xWindow="3690" yWindow="0" windowWidth="16605" windowHeight="10920" firstSheet="3" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="OCTUBRE      2 0 2 1     " sheetId="1" r:id="rId1"/>
@@ -211,7 +211,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="315">
   <si>
     <t>COMPRAS</t>
   </si>
@@ -1153,6 +1153,9 @@
   </si>
   <si>
     <t>C-3948</t>
+  </si>
+  <si>
+    <t>DEBE  ZAVALETA</t>
   </si>
 </sst>
 </file>
@@ -2826,7 +2829,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="448">
+  <cellXfs count="450">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -3600,6 +3603,42 @@
     <xf numFmtId="164" fontId="3" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="3" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3672,45 +3711,60 @@
     <xf numFmtId="44" fontId="12" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="1" fontId="43" fillId="6" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="43" fillId="6" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="57" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="77" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="58" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="59" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="16" fillId="3" borderId="69" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="16" fillId="3" borderId="71" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="3" borderId="70" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="3" borderId="72" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="41" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="41" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="44" fontId="13" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3738,54 +3792,6 @@
     <xf numFmtId="7" fontId="11" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="57" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="77" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="58" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="59" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="16" fillId="3" borderId="69" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="16" fillId="3" borderId="71" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="3" borderId="70" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="3" borderId="72" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="41" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="41" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="44" fontId="3" fillId="3" borderId="74" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3798,8 +3804,11 @@
     <xf numFmtId="44" fontId="2" fillId="17" borderId="82" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="164" fontId="33" fillId="7" borderId="80" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="33" fillId="7" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -5403,23 +5412,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="405"/>
-      <c r="C1" s="407" t="s">
+      <c r="B1" s="382"/>
+      <c r="C1" s="384" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="408"/>
-      <c r="E1" s="408"/>
-      <c r="F1" s="408"/>
-      <c r="G1" s="408"/>
-      <c r="H1" s="408"/>
-      <c r="I1" s="408"/>
-      <c r="J1" s="408"/>
-      <c r="K1" s="408"/>
-      <c r="L1" s="408"/>
-      <c r="M1" s="408"/>
+      <c r="D1" s="385"/>
+      <c r="E1" s="385"/>
+      <c r="F1" s="385"/>
+      <c r="G1" s="385"/>
+      <c r="H1" s="385"/>
+      <c r="I1" s="385"/>
+      <c r="J1" s="385"/>
+      <c r="K1" s="385"/>
+      <c r="L1" s="385"/>
+      <c r="M1" s="385"/>
     </row>
     <row r="2" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="406"/>
+      <c r="B2" s="383"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -5429,17 +5438,17 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:19" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="409" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="410"/>
+      <c r="B3" s="386" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="387"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="411" t="s">
+      <c r="H3" s="388" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="411"/>
+      <c r="I3" s="388"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
@@ -5453,14 +5462,14 @@
         <v>0</v>
       </c>
       <c r="D4" s="18"/>
-      <c r="E4" s="412" t="s">
+      <c r="E4" s="389" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="413"/>
-      <c r="H4" s="414" t="s">
+      <c r="F4" s="390"/>
+      <c r="H4" s="391" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="415"/>
+      <c r="I4" s="392"/>
       <c r="J4" s="19"/>
       <c r="K4" s="166"/>
       <c r="L4" s="20"/>
@@ -5470,10 +5479,10 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="386" t="s">
+      <c r="P4" s="398" t="s">
         <v>6</v>
       </c>
-      <c r="Q4" s="387"/>
+      <c r="Q4" s="399"/>
     </row>
     <row r="5" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="23" t="s">
@@ -6914,11 +6923,11 @@
       <c r="J39" s="60"/>
       <c r="K39" s="177"/>
       <c r="L39" s="61"/>
-      <c r="M39" s="388">
+      <c r="M39" s="400">
         <f>SUM(M5:M38)</f>
         <v>247061</v>
       </c>
-      <c r="N39" s="390">
+      <c r="N39" s="402">
         <f>SUM(N5:N38)</f>
         <v>172863</v>
       </c>
@@ -6944,8 +6953,8 @@
       <c r="J40" s="60"/>
       <c r="K40" s="41"/>
       <c r="L40" s="61"/>
-      <c r="M40" s="389"/>
-      <c r="N40" s="391"/>
+      <c r="M40" s="401"/>
+      <c r="N40" s="403"/>
       <c r="P40" s="34"/>
       <c r="Q40" s="9"/>
     </row>
@@ -7160,29 +7169,29 @@
       <c r="A52" s="98"/>
       <c r="B52" s="99"/>
       <c r="C52" s="1"/>
-      <c r="H52" s="392" t="s">
+      <c r="H52" s="404" t="s">
         <v>11</v>
       </c>
-      <c r="I52" s="393"/>
+      <c r="I52" s="405"/>
       <c r="J52" s="100"/>
-      <c r="K52" s="394">
+      <c r="K52" s="406">
         <f>I50+L50</f>
         <v>53873.49</v>
       </c>
-      <c r="L52" s="395"/>
-      <c r="M52" s="396">
+      <c r="L52" s="407"/>
+      <c r="M52" s="408">
         <f>N39+M39</f>
         <v>419924</v>
       </c>
-      <c r="N52" s="397"/>
+      <c r="N52" s="409"/>
       <c r="P52" s="34"/>
       <c r="Q52" s="9"/>
     </row>
     <row r="53" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D53" s="398" t="s">
+      <c r="D53" s="410" t="s">
         <v>12</v>
       </c>
-      <c r="E53" s="398"/>
+      <c r="E53" s="410"/>
       <c r="F53" s="101">
         <f>F50-K52-C50</f>
         <v>471038.61</v>
@@ -7193,22 +7202,22 @@
       <c r="Q53" s="9"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="398" t="s">
+      <c r="D54" s="410" t="s">
         <v>95</v>
       </c>
-      <c r="E54" s="398"/>
+      <c r="E54" s="410"/>
       <c r="F54" s="96">
         <v>-549976.4</v>
       </c>
-      <c r="I54" s="399" t="s">
+      <c r="I54" s="411" t="s">
         <v>13</v>
       </c>
-      <c r="J54" s="400"/>
-      <c r="K54" s="401">
+      <c r="J54" s="412"/>
+      <c r="K54" s="413">
         <f>F56+F57+F58</f>
         <v>-24577.400000000023</v>
       </c>
-      <c r="L54" s="402"/>
+      <c r="L54" s="414"/>
       <c r="P54" s="34"/>
       <c r="Q54" s="9"/>
     </row>
@@ -7241,11 +7250,11 @@
         <v>15</v>
       </c>
       <c r="J56" s="109"/>
-      <c r="K56" s="403">
+      <c r="K56" s="415">
         <f>-C4</f>
         <v>0</v>
       </c>
-      <c r="L56" s="404"/>
+      <c r="L56" s="416"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="110" t="s">
@@ -7262,22 +7271,22 @@
       <c r="C58" s="112">
         <v>44507</v>
       </c>
-      <c r="D58" s="381" t="s">
+      <c r="D58" s="393" t="s">
         <v>18</v>
       </c>
-      <c r="E58" s="382"/>
+      <c r="E58" s="394"/>
       <c r="F58" s="113">
         <v>567389.35</v>
       </c>
-      <c r="I58" s="383" t="s">
+      <c r="I58" s="395" t="s">
         <v>97</v>
       </c>
-      <c r="J58" s="384"/>
-      <c r="K58" s="385">
+      <c r="J58" s="396"/>
+      <c r="K58" s="397">
         <f>K54+K56</f>
         <v>-24577.400000000023</v>
       </c>
-      <c r="L58" s="385"/>
+      <c r="L58" s="397"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="114"/>
@@ -7421,12 +7430,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
     <mergeCell ref="D58:E58"/>
     <mergeCell ref="I58:J58"/>
     <mergeCell ref="K58:L58"/>
@@ -7441,6 +7444,12 @@
     <mergeCell ref="I54:J54"/>
     <mergeCell ref="K54:L54"/>
     <mergeCell ref="K56:L56"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
   </mergeCells>
   <pageMargins left="0.39370078740157483" right="0.15748031496062992" top="0.35433070866141736" bottom="0.31496062992125984" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="75" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -8781,7 +8790,7 @@
       <c r="A41" s="140">
         <v>44507</v>
       </c>
-      <c r="B41" s="416" t="s">
+      <c r="B41" s="417" t="s">
         <v>92</v>
       </c>
       <c r="C41" s="190">
@@ -8813,7 +8822,7 @@
       <c r="A42" s="140" t="s">
         <v>93</v>
       </c>
-      <c r="B42" s="417"/>
+      <c r="B42" s="418"/>
       <c r="C42" s="143">
         <v>0</v>
       </c>
@@ -10409,23 +10418,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="405"/>
-      <c r="C1" s="407" t="s">
+      <c r="B1" s="382"/>
+      <c r="C1" s="384" t="s">
         <v>208</v>
       </c>
-      <c r="D1" s="408"/>
-      <c r="E1" s="408"/>
-      <c r="F1" s="408"/>
-      <c r="G1" s="408"/>
-      <c r="H1" s="408"/>
-      <c r="I1" s="408"/>
-      <c r="J1" s="408"/>
-      <c r="K1" s="408"/>
-      <c r="L1" s="408"/>
-      <c r="M1" s="408"/>
+      <c r="D1" s="385"/>
+      <c r="E1" s="385"/>
+      <c r="F1" s="385"/>
+      <c r="G1" s="385"/>
+      <c r="H1" s="385"/>
+      <c r="I1" s="385"/>
+      <c r="J1" s="385"/>
+      <c r="K1" s="385"/>
+      <c r="L1" s="385"/>
+      <c r="M1" s="385"/>
     </row>
     <row r="2" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="406"/>
+      <c r="B2" s="383"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -10435,21 +10444,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:25" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="409" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="410"/>
+      <c r="B3" s="386" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="387"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="411" t="s">
+      <c r="H3" s="388" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="411"/>
+      <c r="I3" s="388"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="P3" s="435" t="s">
+      <c r="P3" s="425" t="s">
         <v>6</v>
       </c>
     </row>
@@ -10464,14 +10473,14 @@
       <c r="D4" s="18">
         <v>44507</v>
       </c>
-      <c r="E4" s="412" t="s">
+      <c r="E4" s="389" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="413"/>
-      <c r="H4" s="414" t="s">
+      <c r="F4" s="390"/>
+      <c r="H4" s="391" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="415"/>
+      <c r="I4" s="392"/>
       <c r="J4" s="19"/>
       <c r="K4" s="166"/>
       <c r="L4" s="20"/>
@@ -10481,14 +10490,14 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="436"/>
+      <c r="P4" s="426"/>
       <c r="Q4" s="286" t="s">
         <v>209</v>
       </c>
-      <c r="W4" s="418" t="s">
+      <c r="W4" s="435" t="s">
         <v>124</v>
       </c>
-      <c r="X4" s="418"/>
+      <c r="X4" s="435"/>
       <c r="Y4" s="227"/>
     </row>
     <row r="5" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -10539,8 +10548,8 @@
         <f>20000+7936</f>
         <v>27936</v>
       </c>
-      <c r="W5" s="418"/>
-      <c r="X5" s="418"/>
+      <c r="W5" s="435"/>
+      <c r="X5" s="435"/>
       <c r="Y5" s="233"/>
     </row>
     <row r="6" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -11311,7 +11320,7 @@
         <v>26370</v>
       </c>
       <c r="S19" s="147"/>
-      <c r="W19" s="422">
+      <c r="W19" s="439">
         <f t="shared" ref="W19" si="3">SUM(W6:W18)</f>
         <v>935136</v>
       </c>
@@ -11363,7 +11372,7 @@
         <v>16395.830000000002</v>
       </c>
       <c r="S20" s="147"/>
-      <c r="W20" s="423"/>
+      <c r="W20" s="440"/>
       <c r="X20" s="268"/>
       <c r="Y20" s="233"/>
     </row>
@@ -11412,8 +11421,8 @@
         <v>19188.82</v>
       </c>
       <c r="S21" s="147"/>
-      <c r="W21" s="424"/>
-      <c r="X21" s="424"/>
+      <c r="W21" s="441"/>
+      <c r="X21" s="441"/>
       <c r="Y21" s="233"/>
       <c r="Z21" s="128"/>
     </row>
@@ -11514,8 +11523,8 @@
         <v>45217.29</v>
       </c>
       <c r="S23" s="147"/>
-      <c r="W23" s="425"/>
-      <c r="X23" s="425"/>
+      <c r="W23" s="442"/>
+      <c r="X23" s="442"/>
       <c r="Y23" s="233"/>
       <c r="Z23" s="128"/>
     </row>
@@ -11569,8 +11578,8 @@
         <v>23159.17</v>
       </c>
       <c r="S24" s="147"/>
-      <c r="W24" s="425"/>
-      <c r="X24" s="425"/>
+      <c r="W24" s="442"/>
+      <c r="X24" s="442"/>
       <c r="Y24" s="233"/>
       <c r="Z24" s="128"/>
     </row>
@@ -11616,8 +11625,8 @@
       <c r="R25" s="285">
         <v>28952</v>
       </c>
-      <c r="W25" s="426"/>
-      <c r="X25" s="426"/>
+      <c r="W25" s="443"/>
+      <c r="X25" s="443"/>
       <c r="Y25" s="233"/>
       <c r="Z25" s="128"/>
     </row>
@@ -11668,8 +11677,8 @@
       <c r="R26" s="285">
         <v>21771.5</v>
       </c>
-      <c r="W26" s="426"/>
-      <c r="X26" s="426"/>
+      <c r="W26" s="443"/>
+      <c r="X26" s="443"/>
       <c r="Y26" s="233"/>
       <c r="Z26" s="128"/>
     </row>
@@ -11717,9 +11726,9 @@
       <c r="R27" s="285">
         <v>14637</v>
       </c>
-      <c r="W27" s="419"/>
-      <c r="X27" s="420"/>
-      <c r="Y27" s="421"/>
+      <c r="W27" s="436"/>
+      <c r="X27" s="437"/>
+      <c r="Y27" s="438"/>
       <c r="Z27" s="128"/>
     </row>
     <row r="28" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -11769,9 +11778,9 @@
       <c r="R28" s="285">
         <v>0</v>
       </c>
-      <c r="W28" s="420"/>
-      <c r="X28" s="420"/>
-      <c r="Y28" s="421"/>
+      <c r="W28" s="437"/>
+      <c r="X28" s="437"/>
+      <c r="Y28" s="438"/>
       <c r="Z28" s="128"/>
     </row>
     <row r="29" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -12106,11 +12115,11 @@
       <c r="L36" s="44">
         <v>5940</v>
       </c>
-      <c r="M36" s="437">
+      <c r="M36" s="427">
         <f t="shared" ref="M36" si="4">SUM(M5:M35)</f>
         <v>321168.83</v>
       </c>
-      <c r="N36" s="439">
+      <c r="N36" s="429">
         <f t="shared" ref="N36" si="5">SUM(N5:N35)</f>
         <v>467016</v>
       </c>
@@ -12118,7 +12127,7 @@
       <c r="P36" s="277">
         <v>0</v>
       </c>
-      <c r="Q36" s="441">
+      <c r="Q36" s="431">
         <f t="shared" ref="Q36" si="6">SUM(Q5:Q35)</f>
         <v>-637069.14000000013</v>
       </c>
@@ -12153,13 +12162,13 @@
       <c r="L37" s="61">
         <v>7929.62</v>
       </c>
-      <c r="M37" s="438"/>
-      <c r="N37" s="440"/>
+      <c r="M37" s="428"/>
+      <c r="N37" s="430"/>
       <c r="O37" s="276"/>
       <c r="P37" s="277">
         <v>0</v>
       </c>
-      <c r="Q37" s="442"/>
+      <c r="Q37" s="432"/>
     </row>
     <row r="38" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="23"/>
@@ -12449,26 +12458,26 @@
       <c r="A52" s="98"/>
       <c r="B52" s="99"/>
       <c r="C52" s="1"/>
-      <c r="H52" s="392" t="s">
+      <c r="H52" s="404" t="s">
         <v>11</v>
       </c>
-      <c r="I52" s="393"/>
+      <c r="I52" s="405"/>
       <c r="J52" s="100"/>
-      <c r="K52" s="394">
+      <c r="K52" s="406">
         <f>I50+L50</f>
         <v>71911.59</v>
       </c>
-      <c r="L52" s="427"/>
+      <c r="L52" s="433"/>
       <c r="M52" s="272"/>
       <c r="N52" s="272"/>
       <c r="P52" s="34"/>
       <c r="Q52" s="13"/>
     </row>
     <row r="53" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D53" s="398" t="s">
+      <c r="D53" s="410" t="s">
         <v>12</v>
       </c>
-      <c r="E53" s="398"/>
+      <c r="E53" s="410"/>
       <c r="F53" s="313">
         <f>F50-K52-C50</f>
         <v>-25952.549999999814</v>
@@ -12477,29 +12486,29 @@
       <c r="J53" s="103"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="428" t="s">
+      <c r="D54" s="434" t="s">
         <v>95</v>
       </c>
-      <c r="E54" s="428"/>
+      <c r="E54" s="434"/>
       <c r="F54" s="111">
         <v>-706888.38</v>
       </c>
-      <c r="I54" s="399" t="s">
+      <c r="I54" s="411" t="s">
         <v>13</v>
       </c>
-      <c r="J54" s="400"/>
-      <c r="K54" s="401">
+      <c r="J54" s="412"/>
+      <c r="K54" s="413">
         <f>F56+F57+F58</f>
         <v>1308778.3500000003</v>
       </c>
-      <c r="L54" s="401"/>
-      <c r="M54" s="429" t="s">
+      <c r="L54" s="413"/>
+      <c r="M54" s="419" t="s">
         <v>211</v>
       </c>
-      <c r="N54" s="430"/>
-      <c r="O54" s="430"/>
-      <c r="P54" s="430"/>
-      <c r="Q54" s="431"/>
+      <c r="N54" s="420"/>
+      <c r="O54" s="420"/>
+      <c r="P54" s="420"/>
+      <c r="Q54" s="421"/>
     </row>
     <row r="55" spans="1:17" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D55" s="314" t="s">
@@ -12513,11 +12522,11 @@
       <c r="J55" s="106"/>
       <c r="K55" s="178"/>
       <c r="L55" s="107"/>
-      <c r="M55" s="432"/>
-      <c r="N55" s="433"/>
-      <c r="O55" s="433"/>
-      <c r="P55" s="433"/>
-      <c r="Q55" s="434"/>
+      <c r="M55" s="422"/>
+      <c r="N55" s="423"/>
+      <c r="O55" s="423"/>
+      <c r="P55" s="423"/>
+      <c r="Q55" s="424"/>
     </row>
     <row r="56" spans="1:17" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
       <c r="C56" s="4" t="s">
@@ -12535,11 +12544,11 @@
         <v>15</v>
       </c>
       <c r="J56" s="109"/>
-      <c r="K56" s="403">
+      <c r="K56" s="415">
         <f>-C4</f>
         <v>-567389.35</v>
       </c>
-      <c r="L56" s="404"/>
+      <c r="L56" s="416"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="110" t="s">
@@ -12556,22 +12565,22 @@
       <c r="C58" s="112">
         <v>44535</v>
       </c>
-      <c r="D58" s="381" t="s">
+      <c r="D58" s="393" t="s">
         <v>18</v>
       </c>
-      <c r="E58" s="382"/>
+      <c r="E58" s="394"/>
       <c r="F58" s="113">
         <v>2142307.62</v>
       </c>
-      <c r="I58" s="383" t="s">
+      <c r="I58" s="395" t="s">
         <v>198</v>
       </c>
-      <c r="J58" s="384"/>
-      <c r="K58" s="385">
+      <c r="J58" s="396"/>
+      <c r="K58" s="397">
         <f>K54+K56</f>
         <v>741389.00000000035</v>
       </c>
-      <c r="L58" s="385"/>
+      <c r="L58" s="397"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="114"/>
@@ -12715,17 +12724,14 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="M54:Q55"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="M36:M37"/>
-    <mergeCell ref="N36:N37"/>
-    <mergeCell ref="Q36:Q37"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="W4:X5"/>
+    <mergeCell ref="W27:X28"/>
+    <mergeCell ref="Y27:Y28"/>
+    <mergeCell ref="W19:W20"/>
+    <mergeCell ref="W21:X21"/>
+    <mergeCell ref="W23:X24"/>
+    <mergeCell ref="W25:X25"/>
+    <mergeCell ref="W26:X26"/>
     <mergeCell ref="D58:E58"/>
     <mergeCell ref="I58:J58"/>
     <mergeCell ref="K58:L58"/>
@@ -12736,14 +12742,17 @@
     <mergeCell ref="I54:J54"/>
     <mergeCell ref="K54:L54"/>
     <mergeCell ref="K56:L56"/>
-    <mergeCell ref="W4:X5"/>
-    <mergeCell ref="W27:X28"/>
-    <mergeCell ref="Y27:Y28"/>
-    <mergeCell ref="W19:W20"/>
-    <mergeCell ref="W21:X21"/>
-    <mergeCell ref="W23:X24"/>
-    <mergeCell ref="W25:X25"/>
-    <mergeCell ref="W26:X26"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="M54:Q55"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="M36:M37"/>
+    <mergeCell ref="N36:N37"/>
+    <mergeCell ref="Q36:Q37"/>
   </mergeCells>
   <pageMargins left="0.15748031496062992" right="0.15748031496062992" top="0.27559055118110237" bottom="0.27559055118110237" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="68" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -12759,8 +12768,8 @@
   </sheetPr>
   <dimension ref="A1:N122"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="F92" sqref="F92"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D90" sqref="D90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15161,7 +15170,7 @@
       <c r="C87" s="214"/>
       <c r="D87" s="97"/>
       <c r="E87" s="3"/>
-      <c r="F87" s="443" t="s">
+      <c r="F87" s="444" t="s">
         <v>207</v>
       </c>
       <c r="K87" s="1"/>
@@ -15174,7 +15183,7 @@
       <c r="C88" s="1"/>
       <c r="D88" s="97"/>
       <c r="E88" s="3"/>
-      <c r="F88" s="444"/>
+      <c r="F88" s="445"/>
       <c r="K88" s="1"/>
       <c r="L88" s="256"/>
       <c r="M88" s="3"/>
@@ -15486,23 +15495,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="405"/>
-      <c r="C1" s="407" t="s">
+      <c r="B1" s="382"/>
+      <c r="C1" s="384" t="s">
         <v>208</v>
       </c>
-      <c r="D1" s="408"/>
-      <c r="E1" s="408"/>
-      <c r="F1" s="408"/>
-      <c r="G1" s="408"/>
-      <c r="H1" s="408"/>
-      <c r="I1" s="408"/>
-      <c r="J1" s="408"/>
-      <c r="K1" s="408"/>
-      <c r="L1" s="408"/>
-      <c r="M1" s="408"/>
+      <c r="D1" s="385"/>
+      <c r="E1" s="385"/>
+      <c r="F1" s="385"/>
+      <c r="G1" s="385"/>
+      <c r="H1" s="385"/>
+      <c r="I1" s="385"/>
+      <c r="J1" s="385"/>
+      <c r="K1" s="385"/>
+      <c r="L1" s="385"/>
+      <c r="M1" s="385"/>
     </row>
     <row r="2" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="406"/>
+      <c r="B2" s="383"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -15512,24 +15521,24 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:25" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="409" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="410"/>
+      <c r="B3" s="386" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="387"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="411" t="s">
+      <c r="H3" s="388" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="411"/>
+      <c r="I3" s="388"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="P3" s="435" t="s">
+      <c r="P3" s="425" t="s">
         <v>6</v>
       </c>
-      <c r="R3" s="445" t="s">
+      <c r="R3" s="446" t="s">
         <v>216</v>
       </c>
     </row>
@@ -15544,14 +15553,14 @@
       <c r="D4" s="18">
         <v>44507</v>
       </c>
-      <c r="E4" s="412" t="s">
+      <c r="E4" s="389" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="413"/>
-      <c r="H4" s="414" t="s">
+      <c r="F4" s="390"/>
+      <c r="H4" s="391" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="415"/>
+      <c r="I4" s="392"/>
       <c r="J4" s="19"/>
       <c r="K4" s="166"/>
       <c r="L4" s="20"/>
@@ -15561,15 +15570,15 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="436"/>
+      <c r="P4" s="426"/>
       <c r="Q4" s="323" t="s">
         <v>217</v>
       </c>
-      <c r="R4" s="446"/>
-      <c r="W4" s="418" t="s">
+      <c r="R4" s="447"/>
+      <c r="W4" s="435" t="s">
         <v>124</v>
       </c>
-      <c r="X4" s="418"/>
+      <c r="X4" s="435"/>
       <c r="Y4" s="227"/>
     </row>
     <row r="5" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -15630,8 +15639,8 @@
       <c r="S5" s="325" t="s">
         <v>213</v>
       </c>
-      <c r="W5" s="418"/>
-      <c r="X5" s="418"/>
+      <c r="W5" s="435"/>
+      <c r="X5" s="435"/>
       <c r="Y5" s="233"/>
     </row>
     <row r="6" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -16388,7 +16397,7 @@
         <v>0</v>
       </c>
       <c r="S19" s="147"/>
-      <c r="W19" s="422">
+      <c r="W19" s="439">
         <f t="shared" ref="W19" si="3">SUM(W6:W18)</f>
         <v>0</v>
       </c>
@@ -16440,7 +16449,7 @@
         <v>0</v>
       </c>
       <c r="S20" s="147"/>
-      <c r="W20" s="423"/>
+      <c r="W20" s="440"/>
       <c r="X20" s="268"/>
       <c r="Y20" s="233"/>
     </row>
@@ -16489,8 +16498,8 @@
         <v>0</v>
       </c>
       <c r="S21" s="147"/>
-      <c r="W21" s="424"/>
-      <c r="X21" s="424"/>
+      <c r="W21" s="441"/>
+      <c r="X21" s="441"/>
       <c r="Y21" s="233"/>
       <c r="Z21" s="128"/>
     </row>
@@ -16591,8 +16600,8 @@
         <v>0</v>
       </c>
       <c r="S23" s="147"/>
-      <c r="W23" s="425"/>
-      <c r="X23" s="425"/>
+      <c r="W23" s="442"/>
+      <c r="X23" s="442"/>
       <c r="Y23" s="233"/>
       <c r="Z23" s="128"/>
     </row>
@@ -16643,8 +16652,8 @@
         <v>0</v>
       </c>
       <c r="S24" s="147"/>
-      <c r="W24" s="425"/>
-      <c r="X24" s="425"/>
+      <c r="W24" s="442"/>
+      <c r="X24" s="442"/>
       <c r="Y24" s="233"/>
       <c r="Z24" s="128"/>
     </row>
@@ -16690,8 +16699,8 @@
       <c r="R25" s="320">
         <v>0</v>
       </c>
-      <c r="W25" s="426"/>
-      <c r="X25" s="426"/>
+      <c r="W25" s="443"/>
+      <c r="X25" s="443"/>
       <c r="Y25" s="233"/>
       <c r="Z25" s="128"/>
     </row>
@@ -16739,8 +16748,8 @@
       <c r="R26" s="320">
         <v>0</v>
       </c>
-      <c r="W26" s="426"/>
-      <c r="X26" s="426"/>
+      <c r="W26" s="443"/>
+      <c r="X26" s="443"/>
       <c r="Y26" s="233"/>
       <c r="Z26" s="128"/>
     </row>
@@ -16800,9 +16809,9 @@
       <c r="V27" t="s">
         <v>240</v>
       </c>
-      <c r="W27" s="419"/>
-      <c r="X27" s="420"/>
-      <c r="Y27" s="421"/>
+      <c r="W27" s="436"/>
+      <c r="X27" s="437"/>
+      <c r="Y27" s="438"/>
       <c r="Z27" s="128"/>
     </row>
     <row r="28" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -16856,9 +16865,9 @@
       <c r="V28" t="s">
         <v>240</v>
       </c>
-      <c r="W28" s="420"/>
-      <c r="X28" s="420"/>
-      <c r="Y28" s="421"/>
+      <c r="W28" s="437"/>
+      <c r="X28" s="437"/>
+      <c r="Y28" s="438"/>
       <c r="Z28" s="128"/>
     </row>
     <row r="29" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -17165,11 +17174,11 @@
       <c r="J36" s="266"/>
       <c r="K36" s="250"/>
       <c r="L36" s="44"/>
-      <c r="M36" s="437">
+      <c r="M36" s="427">
         <f t="shared" ref="M36" si="4">SUM(M5:M35)</f>
         <v>1054774.3</v>
       </c>
-      <c r="N36" s="439">
+      <c r="N36" s="429">
         <f t="shared" ref="N36" si="5">SUM(N5:N35)</f>
         <v>936398</v>
       </c>
@@ -17177,7 +17186,7 @@
       <c r="P36" s="277">
         <v>0</v>
       </c>
-      <c r="Q36" s="441">
+      <c r="Q36" s="431">
         <f t="shared" ref="Q36" si="6">SUM(Q5:Q35)</f>
         <v>-37279.94</v>
       </c>
@@ -17196,13 +17205,13 @@
       <c r="J37" s="60"/>
       <c r="K37" s="41"/>
       <c r="L37" s="61"/>
-      <c r="M37" s="438"/>
-      <c r="N37" s="440"/>
+      <c r="M37" s="428"/>
+      <c r="N37" s="430"/>
       <c r="O37" s="276"/>
       <c r="P37" s="277">
         <v>0</v>
       </c>
-      <c r="Q37" s="442"/>
+      <c r="Q37" s="432"/>
     </row>
     <row r="38" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="23"/>
@@ -17476,26 +17485,26 @@
       <c r="A52" s="98"/>
       <c r="B52" s="99"/>
       <c r="C52" s="1"/>
-      <c r="H52" s="392" t="s">
+      <c r="H52" s="404" t="s">
         <v>11</v>
       </c>
-      <c r="I52" s="393"/>
+      <c r="I52" s="405"/>
       <c r="J52" s="100"/>
-      <c r="K52" s="394">
+      <c r="K52" s="406">
         <f>I50+L50</f>
         <v>90750.75</v>
       </c>
-      <c r="L52" s="427"/>
+      <c r="L52" s="433"/>
       <c r="M52" s="272"/>
       <c r="N52" s="272"/>
       <c r="P52" s="34"/>
       <c r="Q52" s="13"/>
     </row>
     <row r="53" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D53" s="398" t="s">
+      <c r="D53" s="410" t="s">
         <v>12</v>
       </c>
-      <c r="E53" s="398"/>
+      <c r="E53" s="410"/>
       <c r="F53" s="313">
         <f>F50-K52-C50</f>
         <v>1957966.13</v>
@@ -17504,29 +17513,29 @@
       <c r="J53" s="103"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="428" t="s">
+      <c r="D54" s="434" t="s">
         <v>95</v>
       </c>
-      <c r="E54" s="428"/>
+      <c r="E54" s="434"/>
       <c r="F54" s="111">
         <v>-1567070.66</v>
       </c>
-      <c r="I54" s="399" t="s">
+      <c r="I54" s="411" t="s">
         <v>13</v>
       </c>
-      <c r="J54" s="400"/>
-      <c r="K54" s="401">
+      <c r="J54" s="412"/>
+      <c r="K54" s="413">
         <f>F56+F57+F58</f>
         <v>921303.96</v>
       </c>
-      <c r="L54" s="401"/>
-      <c r="M54" s="429" t="s">
+      <c r="L54" s="413"/>
+      <c r="M54" s="419" t="s">
         <v>211</v>
       </c>
-      <c r="N54" s="430"/>
-      <c r="O54" s="430"/>
-      <c r="P54" s="430"/>
-      <c r="Q54" s="431"/>
+      <c r="N54" s="420"/>
+      <c r="O54" s="420"/>
+      <c r="P54" s="420"/>
+      <c r="Q54" s="421"/>
     </row>
     <row r="55" spans="1:17" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D55" s="314" t="s">
@@ -17540,11 +17549,11 @@
       <c r="J55" s="106"/>
       <c r="K55" s="178"/>
       <c r="L55" s="107"/>
-      <c r="M55" s="432"/>
-      <c r="N55" s="433"/>
-      <c r="O55" s="433"/>
-      <c r="P55" s="433"/>
-      <c r="Q55" s="434"/>
+      <c r="M55" s="422"/>
+      <c r="N55" s="423"/>
+      <c r="O55" s="423"/>
+      <c r="P55" s="423"/>
+      <c r="Q55" s="424"/>
     </row>
     <row r="56" spans="1:17" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
       <c r="C56" s="4" t="s">
@@ -17562,11 +17571,11 @@
         <v>15</v>
       </c>
       <c r="J56" s="109"/>
-      <c r="K56" s="403">
+      <c r="K56" s="415">
         <f>-C4</f>
         <v>-567389.35</v>
       </c>
-      <c r="L56" s="404"/>
+      <c r="L56" s="416"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="110" t="s">
@@ -17583,22 +17592,22 @@
       <c r="C58" s="112">
         <v>44563</v>
       </c>
-      <c r="D58" s="381" t="s">
+      <c r="D58" s="393" t="s">
         <v>18</v>
       </c>
-      <c r="E58" s="382"/>
+      <c r="E58" s="394"/>
       <c r="F58" s="113">
         <v>754143.23</v>
       </c>
-      <c r="I58" s="383" t="s">
+      <c r="I58" s="395" t="s">
         <v>198</v>
       </c>
-      <c r="J58" s="384"/>
-      <c r="K58" s="385">
+      <c r="J58" s="396"/>
+      <c r="K58" s="397">
         <f>K54+K56</f>
         <v>353914.61</v>
       </c>
-      <c r="L58" s="385"/>
+      <c r="L58" s="397"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="114"/>
@@ -17742,13 +17751,20 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="D58:E58"/>
+    <mergeCell ref="I58:J58"/>
+    <mergeCell ref="K58:L58"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="I54:J54"/>
+    <mergeCell ref="K54:L54"/>
+    <mergeCell ref="M54:Q55"/>
+    <mergeCell ref="K56:L56"/>
+    <mergeCell ref="W27:X28"/>
+    <mergeCell ref="Y27:Y28"/>
+    <mergeCell ref="M36:M37"/>
+    <mergeCell ref="N36:N37"/>
+    <mergeCell ref="Q36:Q37"/>
     <mergeCell ref="H52:I52"/>
     <mergeCell ref="K52:L52"/>
     <mergeCell ref="W4:X5"/>
@@ -17758,20 +17774,13 @@
     <mergeCell ref="W25:X25"/>
     <mergeCell ref="W26:X26"/>
     <mergeCell ref="R3:R4"/>
-    <mergeCell ref="M54:Q55"/>
-    <mergeCell ref="K56:L56"/>
-    <mergeCell ref="W27:X28"/>
-    <mergeCell ref="Y27:Y28"/>
-    <mergeCell ref="M36:M37"/>
-    <mergeCell ref="N36:N37"/>
-    <mergeCell ref="Q36:Q37"/>
-    <mergeCell ref="D58:E58"/>
-    <mergeCell ref="I58:J58"/>
-    <mergeCell ref="K58:L58"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="I54:J54"/>
-    <mergeCell ref="K54:L54"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -17787,8 +17796,8 @@
   </sheetPr>
   <dimension ref="A1:N110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="D77" sqref="D77"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="F81" sqref="E81:F81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17808,7 +17817,7 @@
     <col min="14" max="14" width="19.5703125" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="36.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="43.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="290" t="s">
         <v>90</v>
       </c>
@@ -17816,8 +17825,8 @@
       <c r="C1" s="292"/>
       <c r="D1" s="376"/>
       <c r="E1" s="292"/>
-      <c r="F1" s="158" t="s">
-        <v>27</v>
+      <c r="F1" s="449" t="s">
+        <v>314</v>
       </c>
       <c r="I1" s="301" t="s">
         <v>91</v>
@@ -17826,8 +17835,8 @@
       <c r="K1" s="303"/>
       <c r="L1" s="304"/>
       <c r="M1" s="303"/>
-      <c r="N1" s="305" t="s">
-        <v>27</v>
+      <c r="N1" s="448" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="21.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -18745,7 +18754,7 @@
       <c r="C27" s="96">
         <v>634.5</v>
       </c>
-      <c r="D27" s="447">
+      <c r="D27" s="381">
         <v>44550</v>
       </c>
       <c r="E27" s="96">
@@ -19954,7 +19963,7 @@
       <c r="C75" s="214"/>
       <c r="D75" s="256"/>
       <c r="E75" s="3"/>
-      <c r="F75" s="443" t="s">
+      <c r="F75" s="444" t="s">
         <v>207</v>
       </c>
       <c r="K75" s="1"/>
@@ -19967,7 +19976,7 @@
       <c r="C76" s="1"/>
       <c r="D76" s="256"/>
       <c r="E76" s="3"/>
-      <c r="F76" s="444"/>
+      <c r="F76" s="445"/>
       <c r="K76" s="1"/>
       <c r="L76" s="97"/>
       <c r="M76" s="3"/>
@@ -20237,8 +20246,8 @@
   <mergeCells count="1">
     <mergeCell ref="F75:F76"/>
   </mergeCells>
-  <pageMargins left="0.36" right="0.25" top="0.43" bottom="0.37" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.35433070866141736" right="0.23622047244094491" top="0.43307086614173229" bottom="0.35433070866141736" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup scale="90" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>